<commit_message>
Minor fixes; finished lab3
</commit_message>
<xml_diff>
--- a/Lab3/Lab3/Debug/results.xlsx
+++ b/Lab3/Lab3/Debug/results.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Without load balancing</t>
   </si>
@@ -38,6 +38,18 @@
   </si>
   <si>
     <t>With load balancing</t>
+  </si>
+  <si>
+    <t>time(s)</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>Speedup</t>
+  </si>
+  <si>
+    <t>SpeedupLB</t>
   </si>
 </sst>
 </file>
@@ -73,8 +85,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -204,21 +219,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$6</c:f>
+              <c:f>Sheet1!$C$3:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2079761</c:v>
+                  <c:v>1.37002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5489029</c:v>
+                  <c:v>3.5270100000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8603463</c:v>
+                  <c:v>5.2553900000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10850029</c:v>
+                  <c:v>6.4890999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -233,11 +248,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="1827982752"/>
-        <c:axId val="1827993632"/>
+        <c:axId val="-349309792"/>
+        <c:axId val="-349315232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1827982752"/>
+        <c:axId val="-349309792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -280,7 +295,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1827993632"/>
+        <c:crossAx val="-349315232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -288,7 +303,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1827993632"/>
+        <c:axId val="-349315232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -339,7 +354,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1827982752"/>
+        <c:crossAx val="-349309792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -505,21 +520,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$B$13</c:f>
+              <c:f>Sheet1!$C$10:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8718657</c:v>
+                  <c:v>5.4816900000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8860677</c:v>
+                  <c:v>5.5274999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8729077</c:v>
+                  <c:v>5.5132599999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8792264</c:v>
+                  <c:v>5.5763100000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -534,11 +549,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="1827992544"/>
-        <c:axId val="1827981120"/>
+        <c:axId val="-349303808"/>
+        <c:axId val="-349314688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1827992544"/>
+        <c:axId val="-349303808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,7 +596,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1827981120"/>
+        <c:crossAx val="-349314688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -589,9 +604,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1827981120"/>
+        <c:axId val="-349314688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="7"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -640,7 +657,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1827992544"/>
+        <c:crossAx val="-349303808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2131,105 +2148,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>2079761</v>
       </c>
+      <c r="C3">
+        <v>1.37002</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <v>5489029</v>
       </c>
+      <c r="C4">
+        <v>3.5270100000000002</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>8603463</v>
       </c>
+      <c r="C5">
+        <v>5.2553900000000002</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>10850029</v>
       </c>
+      <c r="C6">
+        <v>6.4890999999999996</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10">
         <v>8718657</v>
       </c>
+      <c r="C10">
+        <v>5.4816900000000004</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11">
         <v>8860677</v>
       </c>
+      <c r="C11">
+        <v>5.5274999999999999</v>
+      </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12">
         <v>8729077</v>
       </c>
+      <c r="C12">
+        <v>5.5132599999999998</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13">
         <v>8792264</v>
       </c>
+      <c r="C13">
+        <v>5.5763100000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>10.191000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <f>B19/C6</f>
+        <v>1.570479727543111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <f>B19/C13</f>
+        <v>1.8275526288889965</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A8:C8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>